<commit_message>
20231028 Satuiday Study for 3h10m,I felt a little tired.So play games tonight!
</commit_message>
<xml_diff>
--- a/dairy/自学计划与记录.xlsx
+++ b/dairy/自学计划与记录.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="22368" windowHeight="10007" activeTab="1"/>
+    <workbookView windowWidth="22368" windowHeight="10007"/>
   </bookViews>
   <sheets>
     <sheet name="阶段自学计划" sheetId="3" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="83">
   <si>
     <t>时间</t>
   </si>
@@ -39,7 +39,7 @@
     <t>路由与交换技术</t>
   </si>
   <si>
-    <t>第一周半小时/天，第二周45min/天，第三周一个小时/天，第四周两小时/天</t>
+    <t>第一周半小时/天，第二周45min/天，第三周一个小时/天</t>
   </si>
   <si>
     <t>英语</t>
@@ -61,6 +61,24 @@
   </si>
   <si>
     <t>离散数学</t>
+  </si>
+  <si>
+    <t>《TCP/IP详解》</t>
+  </si>
+  <si>
+    <t>《Wireshark数据包分析实战》</t>
+  </si>
+  <si>
+    <t>《鸟哥的LINUX私房菜·基础学习篇》</t>
+  </si>
+  <si>
+    <t>《图解HTTP》</t>
+  </si>
+  <si>
+    <t>《图解TCP/IP》</t>
+  </si>
+  <si>
+    <t>《图解网络硬件》</t>
   </si>
   <si>
     <t>学习日报</t>
@@ -293,6 +311,75 @@
 4.medium一篇文章，或考研公众号一篇文章，写日记
 5.《网络是怎样连接的》15min
 5.《离散数学》15min</t>
+  </si>
+  <si>
+    <t>1.考研英语阅读文章一篇
+2.《TCP/IP详解》译者序-P1
+3.《Wireshark数据包分析与实战》序-P1
+4.《网络是怎样连接的》P12-P17
+5.《离散数学》P4-P6
+6.《微积分普林斯顿读本》P121-P132
+7.《TCP/IP详解》译者序-P1</t>
+  </si>
+  <si>
+    <t>2023年 10月 26日</t>
+  </si>
+  <si>
+    <t>第一个月第四周231016-231022
+试运行，每天：
+1. 《路由与交换机技术》60min
+2.《微积分普林斯顿读本》30min
+3.《精通Git》30min
+4.medium一篇文章，或考研公众号一篇文章，写日记
+5.《网络是怎样连接的》15min
+5.《离散数学》15min
+6.《TCP/IP详解》10min
+7.《Wireshark数据包分析与实战》10min</t>
+  </si>
+  <si>
+    <t>1.《精通Git》P77-P82
+2.《鸟哥的;INUX私房菜·基础学习篇》序-P3
+3.《图解HTTP》序-P4
+4.《图解TCP/IP》序-P5
+5.《图解网络硬件》序-P3
+6《路由与交换技术》P145-P158
+7.《网络是怎样连接的》P17-P25 
+8.《普林斯顿微积分读本》P132-P145
+9.《Wireshark数据包分析与实战》P1-P6</t>
+  </si>
+  <si>
+    <t>2023年 10月 27日</t>
+  </si>
+  <si>
+    <t>第一个月第四周231016-231022
+试运行，每天：
+1. 《路由与交换机技术》60min
+2.《微积分普林斯顿读本》30min
+3.《精通Git》30min
+4.medium一篇文章，或考研公众号一篇文章，写日记
+5.《网络是怎样连接的》15min
+5.《离散数学》15min
+6.《TCP/IP详解》10min
+7.《Wireshark数据包分析与实战》10min
+8.《图解HTTP》10min
+9.《图解TCP/IP》10min
+10.《图解》网络硬件10min
+11.《鸟哥的LINUX私房菜·基础学习篇》10min</t>
+  </si>
+  <si>
+    <t>1.《精通Git》P82P-P100
+2.《鸟哥的;INUX私房菜·基础学习篇》P3-P6
+3.《图解HTTP》P4-P10
+4.《图解TCP/IP》P5-P8
+5.《图解网络硬件》P3-P8
+6《路由与交换技术》P158-P180
+7.《网络是怎样连接的》P25 -P28
+8.《普林斯顿微积分读本》P145-P156
+9.《Wireshark数据包分析与实战》P6-P10
+10.《离散数学》P6-P8</t>
+  </si>
+  <si>
+    <t>2023年 10月 28日</t>
   </si>
   <si>
     <t>学习周报</t>
@@ -1683,13 +1770,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B7"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8" outlineLevelRow="6" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8" outlineLevelCol="3"/>
   <cols>
     <col min="1" max="1" width="17.7407407407407" customWidth="1"/>
     <col min="2" max="2" width="14.1111111111111" style="27" customWidth="1"/>
@@ -1766,8 +1853,8 @@
       </c>
     </row>
     <row r="7" ht="41.7" customHeight="1" spans="1:4">
-      <c r="A7" s="38"/>
-      <c r="B7" s="39"/>
+      <c r="A7" s="36"/>
+      <c r="B7" s="37"/>
       <c r="C7" s="34" t="s">
         <v>14</v>
       </c>
@@ -1775,10 +1862,70 @@
         <v>11</v>
       </c>
     </row>
+    <row r="8" ht="41.7" customHeight="1" spans="1:4">
+      <c r="A8" s="36"/>
+      <c r="B8" s="37"/>
+      <c r="C8" s="34" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="35" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" ht="41.7" customHeight="1" spans="1:4">
+      <c r="A9" s="36"/>
+      <c r="B9" s="37"/>
+      <c r="C9" s="34" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" s="35" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" ht="41.7" customHeight="1" spans="1:4">
+      <c r="A10" s="36"/>
+      <c r="B10" s="37"/>
+      <c r="C10" s="34" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" s="35" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" ht="41.7" customHeight="1" spans="1:4">
+      <c r="A11" s="36"/>
+      <c r="B11" s="37"/>
+      <c r="C11" s="34" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" s="35" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" ht="41.7" customHeight="1" spans="1:4">
+      <c r="A12" s="36"/>
+      <c r="B12" s="37"/>
+      <c r="C12" s="34" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" s="35" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" ht="41.7" customHeight="1" spans="1:4">
+      <c r="A13" s="38"/>
+      <c r="B13" s="39"/>
+      <c r="C13" s="34" t="s">
+        <v>20</v>
+      </c>
+      <c r="D13" s="35" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A2:A7"/>
-    <mergeCell ref="B2:B7"/>
+    <mergeCell ref="A2:A13"/>
+    <mergeCell ref="B2:B13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>
@@ -1788,10 +1935,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:W22"/>
+  <dimension ref="A1:W25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8"/>
@@ -1804,7 +1951,7 @@
   <sheetData>
     <row r="1" spans="1:23">
       <c r="A1" s="15" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="B1" s="16"/>
       <c r="C1" s="16"/>
@@ -1906,26 +2053,26 @@
     </row>
     <row r="5" ht="36" customHeight="1" spans="1:1">
       <c r="A5" s="21" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" ht="20.4" customHeight="1" spans="1:1">
       <c r="A6" s="8" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" ht="36" customHeight="1" spans="1:4">
       <c r="A7" s="22" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="B7" s="22" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="C7" s="22" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="D7" s="22" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" ht="100.05" customHeight="1" spans="1:4">
@@ -1933,13 +2080,13 @@
         <v>1</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="C8" s="23" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" ht="100.05" customHeight="1" spans="1:4">
@@ -1947,13 +2094,13 @@
         <v>2</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="C9" s="23" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" ht="100.05" customHeight="1" spans="1:4">
@@ -1961,13 +2108,13 @@
         <v>3</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="C10" s="23" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11" ht="100.05" customHeight="1" spans="1:4">
@@ -1975,13 +2122,13 @@
         <v>4</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="C11" s="23" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
     </row>
     <row r="12" ht="100.05" customHeight="1" spans="1:4">
@@ -1989,13 +2136,13 @@
         <v>5</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="C12" s="23" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
     </row>
     <row r="13" ht="100.05" customHeight="1" spans="1:4">
@@ -2003,13 +2150,13 @@
         <v>6</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="C13" s="23" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="D13" s="11" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
     </row>
     <row r="14" ht="100.05" customHeight="1" spans="1:4">
@@ -2017,13 +2164,13 @@
         <v>7</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="C14" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="D14" s="11" t="s">
         <v>37</v>
-      </c>
-      <c r="D14" s="11" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="15" customFormat="1" ht="100.05" customHeight="1" spans="1:4">
@@ -2031,13 +2178,13 @@
         <v>8</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="C15" s="23" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="D15" s="11" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
     </row>
     <row r="16" customFormat="1" ht="100.05" customHeight="1" spans="1:4">
@@ -2045,13 +2192,13 @@
         <v>9</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="C16" s="23" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="D16" s="11" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
     </row>
     <row r="17" customFormat="1" ht="100.05" customHeight="1" spans="1:4">
@@ -2059,13 +2206,13 @@
         <v>10</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="C17" s="23" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="D17" s="11" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
     </row>
     <row r="18" customFormat="1" ht="100.05" customHeight="1" spans="1:4">
@@ -2073,13 +2220,13 @@
         <v>11</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="C18" s="23" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="D18" s="11" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
     </row>
     <row r="19" customFormat="1" ht="100.05" customHeight="1" spans="1:4">
@@ -2087,13 +2234,13 @@
         <v>12</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="C19" s="23" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="D19" s="11" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
     </row>
     <row r="20" customFormat="1" ht="110.4" spans="1:4">
@@ -2101,13 +2248,13 @@
         <v>13</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="C20" s="23" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="D20" s="11" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
     </row>
     <row r="21" customFormat="1" ht="110.4" spans="1:4">
@@ -2115,13 +2262,13 @@
         <v>14</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="C21" s="23" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="D21" s="11" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
     </row>
     <row r="22" customFormat="1" ht="110.4" spans="1:4">
@@ -2129,13 +2276,55 @@
         <v>15</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="C22" s="23" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="D22" s="11" t="s">
-        <v>58</v>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="23" customFormat="1" ht="138" spans="1:4">
+      <c r="A23" s="10">
+        <v>16</v>
+      </c>
+      <c r="B23" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="C23" s="23" t="s">
+        <v>66</v>
+      </c>
+      <c r="D23" s="11" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="24" customFormat="1" ht="193.2" spans="1:4">
+      <c r="A24" s="10">
+        <v>16</v>
+      </c>
+      <c r="B24" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="C24" s="23" t="s">
+        <v>69</v>
+      </c>
+      <c r="D24" s="11" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="25" customFormat="1" ht="193.2" spans="1:4">
+      <c r="A25" s="10">
+        <v>16</v>
+      </c>
+      <c r="B25" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="C25" s="23" t="s">
+        <v>72</v>
+      </c>
+      <c r="D25" s="11" t="s">
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -2152,7 +2341,7 @@
   <sheetPr/>
   <dimension ref="A1:W11"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" topLeftCell="B9" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" topLeftCell="B10" workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
@@ -2166,7 +2355,7 @@
   <sheetData>
     <row r="1" spans="1:23">
       <c r="A1" s="1" t="s">
-        <v>59</v>
+        <v>73</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -2268,26 +2457,26 @@
     </row>
     <row r="5" ht="36" customHeight="1" spans="1:1">
       <c r="A5" s="7" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" ht="30" customHeight="1" spans="1:1">
       <c r="A6" s="8" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" ht="36" customHeight="1" spans="1:4">
       <c r="A7" s="9" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" ht="82.8" spans="1:4">
@@ -2295,13 +2484,13 @@
         <v>1</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>60</v>
+        <v>74</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>61</v>
+        <v>75</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" ht="96.6" spans="1:4">
@@ -2309,13 +2498,13 @@
         <v>2</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>62</v>
+        <v>76</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>63</v>
+        <v>77</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>64</v>
+        <v>78</v>
       </c>
     </row>
     <row r="10" ht="110.4" spans="1:4">
@@ -2323,27 +2512,27 @@
         <v>3</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>65</v>
+        <v>79</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>66</v>
+        <v>80</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="11" ht="110.4" spans="1:4">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="11" ht="193.2" spans="1:4">
       <c r="A11" s="10">
         <v>4</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>65</v>
+        <v>79</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>68</v>
+        <v>82</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>58</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>